<commit_message>
version avec nouveaux bibtex
</commit_message>
<xml_diff>
--- a/Datasets/TestNN/TestNN_pre-extract.xlsx
+++ b/Datasets/TestNN/TestNN_pre-extract.xlsx
@@ -6474,7 +6474,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Introducing ASIL inspired dynamic tactical safety decision framework for automated vehicles</t>
+          <t xml:space="preserve"> Introducing ASIL inspired dynamic tactical safety decision framework for automated vehicles 2</t>
         </is>
       </c>
       <c r="E96" t="inlineStr"/>
@@ -6974,7 +6974,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Virtual Environment for Training Autonomous Vehicles</t>
+          <t>Virtual Environment for Training Autonomous Vehicles 2</t>
         </is>
       </c>
       <c r="E104" t="inlineStr"/>
@@ -7038,7 +7038,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Compositional Falsification of Cyber-Physical Systems with Machine Learning Components</t>
+          <t>Compositional Falsification of Cyber-Physical Systems with Machine Learning Components 2</t>
         </is>
       </c>
       <c r="E105" t="inlineStr"/>
@@ -7098,7 +7098,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Safety Assurance Strategies for Autonomous Vehicles</t>
+          <t>Safety Assurance Strategies for Autonomous Vehicles 2</t>
         </is>
       </c>
       <c r="E106" t="inlineStr"/>
@@ -7854,7 +7854,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Visualizing and understanding convolutional networks</t>
+          <t xml:space="preserve"> Visualizing and understanding convolutional networks 2</t>
         </is>
       </c>
       <c r="E119" t="inlineStr"/>
@@ -8358,7 +8358,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Understanding deep image representations by inverting them</t>
+          <t xml:space="preserve"> Understanding deep image representations by inverting them 2</t>
         </is>
       </c>
       <c r="E128" t="inlineStr"/>
@@ -10006,7 +10006,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>Towards proving the adversarial robustness of deep neural networks</t>
+          <t>Towards proving the adversarial robustness of deep neural networks 2</t>
         </is>
       </c>
       <c r="E157" t="inlineStr"/>

</xml_diff>